<commit_message>
added few more java practice programs
</commit_message>
<xml_diff>
--- a/bin/programList/practicePrograms.xlsx
+++ b/bin/programList/practicePrograms.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="97">
   <si>
     <t>Programs</t>
   </si>
@@ -299,6 +299,18 @@
   </si>
   <si>
     <t>add2Integers.java</t>
+  </si>
+  <si>
+    <t>multiply2Floating.java</t>
+  </si>
+  <si>
+    <t>findASCII.java</t>
+  </si>
+  <si>
+    <t>findQuotientAndRemainder.java</t>
+  </si>
+  <si>
+    <t>swapUsing3Variable.java</t>
   </si>
 </sst>
 </file>
@@ -651,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,29 +710,45 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">

</xml_diff>

<commit_message>
added few more programs 07/24
</commit_message>
<xml_diff>
--- a/bin/programList/practicePrograms.xlsx
+++ b/bin/programList/practicePrograms.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15465" windowHeight="2175"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15000" windowHeight="4050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="104">
   <si>
     <t>Programs</t>
   </si>
@@ -311,6 +311,27 @@
   </si>
   <si>
     <t>swapUsing3Variable.java</t>
+  </si>
+  <si>
+    <t>swapWithout3Variable.java</t>
+  </si>
+  <si>
+    <t>evenOrOdd.java</t>
+  </si>
+  <si>
+    <t>vowelOrConsonant.java</t>
+  </si>
+  <si>
+    <t>positiveOrNegative.java</t>
+  </si>
+  <si>
+    <t>aplhabetOrNot.java</t>
+  </si>
+  <si>
+    <t>sumOfNaturalNumbers.java</t>
+  </si>
+  <si>
+    <t>largestAmongThree.java</t>
   </si>
 </sst>
 </file>
@@ -663,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,29 +775,45 @@
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -796,22 +833,34 @@
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">

</xml_diff>